<commit_message>
modification of balance titles
</commit_message>
<xml_diff>
--- a/src/files/tempPDF/SoldeArmateur.xlsx
+++ b/src/files/tempPDF/SoldeArmateur.xlsx
@@ -12,13 +12,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Édité le : 27/01/2025 à 15:50:54 
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Édité le : 28/01/2025 à 09:16:13 
  par :</t>
   </si>
   <si>
-    <t>Soldes Des Armateurs</t>
+    <t>Solde des Armateurs Créditeurs</t>
   </si>
   <si>
     <t/>
@@ -33,19 +33,16 @@
     <t>SOFIEN AMICH</t>
   </si>
   <si>
-    <t>653,00</t>
-  </si>
-  <si>
     <t>MOHAMED MOHAMED</t>
   </si>
   <si>
-    <t>39 141,00</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>39 794,00 DT</t>
+  </si>
+  <si>
+    <t>Soldes des Armateurs Débiteurs</t>
   </si>
   <si>
     <t>0,00 DT</t>
@@ -55,6 +52,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt formatCode="#,##0.00" numFmtId="164"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -136,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf applyFont="1" fontId="0"/>
     <xf applyFont="1" fontId="1" applyFill="1" fillId="2" applyBorder="1" borderId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -155,6 +155,9 @@
     </xf>
     <xf applyFont="1" fontId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyFont="1" fontId="2" applyBorder="1" borderId="2" applyNumberFormat="1" numFmtId="164" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="1" applyBorder="1" borderId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -216,24 +219,24 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
+      <c r="B6" s="7" t="n">
+        <v>653</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>39141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -266,7 +269,7 @@
     </row>
     <row r="2" spans="1:2" ht="40" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5"/>
     </row>
@@ -290,11 +293,11 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>11</v>
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>